<commit_message>
Add tsv versions of excel files
</commit_message>
<xml_diff>
--- a/tabular/Africa/CosmoAF4miss.xlsx
+++ b/tabular/Africa/CosmoAF4miss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathr\Dropbox\GLUE\Whole clades\Completed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/general/NCBI-RABV-GLUE/tabular/Africa/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63690BD-91C8-4629-B366-D7A4B70C94F7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C95E4-F2D8-7341-B31B-A0DD8F6E6895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20740" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -796,39 +796,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AG10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10"/>
+    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
+      <selection activeCell="I7" sqref="A1:AG10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="22.85546875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="6" max="6" width="22.83203125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="9.1640625" style="1"/>
     <col min="9" max="9" width="9" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
-    <col min="11" max="14" width="9.140625" style="1"/>
-    <col min="15" max="15" width="17.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="14.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5703125" customWidth="1"/>
-    <col min="18" max="18" width="14.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" customWidth="1"/>
-    <col min="20" max="20" width="13.7109375" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" customWidth="1"/>
-    <col min="22" max="22" width="21.140625" customWidth="1"/>
-    <col min="23" max="23" width="23.85546875" customWidth="1"/>
-    <col min="24" max="24" width="23.7109375" style="1" customWidth="1"/>
-    <col min="25" max="25" width="26.42578125" customWidth="1"/>
-    <col min="26" max="26" width="22" style="1" customWidth="1"/>
-    <col min="27" max="27" width="24.7109375" customWidth="1"/>
-    <col min="28" max="29" width="14.28515625" customWidth="1"/>
-    <col min="30" max="32" width="19.85546875" customWidth="1"/>
-    <col min="33" max="33" width="17" customWidth="1"/>
-    <col min="34" max="34" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9.1640625" style="1"/>
+    <col min="15" max="15" width="17.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="14.5" customWidth="1"/>
+    <col min="18" max="18" width="17.5" customWidth="1"/>
+    <col min="19" max="19" width="13.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" customWidth="1"/>
+    <col min="21" max="21" width="21.1640625" customWidth="1"/>
+    <col min="22" max="22" width="23.83203125" customWidth="1"/>
+    <col min="23" max="23" width="23.6640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="26.5" customWidth="1"/>
+    <col min="25" max="25" width="22" style="1" customWidth="1"/>
+    <col min="26" max="26" width="24.6640625" customWidth="1"/>
+    <col min="27" max="28" width="14.33203125" customWidth="1"/>
+    <col min="29" max="31" width="19.83203125" customWidth="1"/>
+    <col min="32" max="32" width="17" customWidth="1"/>
+    <col min="33" max="33" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -874,59 +873,59 @@
       <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="R1" s="3" t="s">
-        <v>15</v>
+        <v>70</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="W1" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="X1" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Z1" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC1" s="3" t="s">
         <v>78</v>
       </c>
+      <c r="AC1" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="AD1" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="AF1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" s="5" t="s">
+      <c r="AG1" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -975,57 +974,57 @@
       <c r="P2" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="Q2" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="R2" s="6" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="V2" s="6">
+        <v>81</v>
+      </c>
+      <c r="U2" s="6">
         <v>1950</v>
       </c>
+      <c r="V2" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="W2" s="6" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z2" s="6">
+        <v>81</v>
+      </c>
+      <c r="Y2" s="6">
         <v>1950</v>
       </c>
+      <c r="Z2" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="AA2" s="6" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD2" s="6"/>
+        <v>81</v>
+      </c>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="AE2" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AF2" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH2" s="14" t="s">
+      <c r="AF2" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG2" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1074,57 +1073,57 @@
       <c r="P3" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="Q3" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="R3" s="7" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="U3" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="V3" s="7">
+        <v>81</v>
+      </c>
+      <c r="U3" s="7">
         <v>1998</v>
       </c>
+      <c r="V3" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="W3" s="7" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="X3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y3" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z3" s="7">
+        <v>81</v>
+      </c>
+      <c r="Y3" s="7">
         <v>1998</v>
       </c>
+      <c r="Z3" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="AA3" s="7" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC3" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD3" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="AC3" s="7"/>
+      <c r="AD3" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="AE3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AF3" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG3" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH3" s="15" t="s">
+      <c r="AF3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG3" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1173,57 +1172,57 @@
       <c r="P4" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="Q4" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="R4" s="8" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="U4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="V4" s="8">
+        <v>81</v>
+      </c>
+      <c r="U4" s="8">
         <v>1999</v>
       </c>
+      <c r="V4" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="W4" s="8" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z4" s="8">
+        <v>81</v>
+      </c>
+      <c r="Y4" s="8">
         <v>1999</v>
       </c>
+      <c r="Z4" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="AA4" s="8" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="AB4" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC4" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD4" s="8"/>
+        <v>81</v>
+      </c>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="AE4" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AF4" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG4" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH4" s="16" t="s">
+      <c r="AF4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG4" s="16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1272,57 +1271,57 @@
       <c r="P5" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="Q5" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="R5" s="7" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="V5" s="7">
+        <v>81</v>
+      </c>
+      <c r="U5" s="7">
         <v>1999</v>
       </c>
+      <c r="V5" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="W5" s="7" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y5" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z5" s="7">
+        <v>81</v>
+      </c>
+      <c r="Y5" s="7">
         <v>1999</v>
       </c>
+      <c r="Z5" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="AA5" s="7" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="AB5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="AC5" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD5" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="AE5" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AF5" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH5" s="15" t="s">
+      <c r="AF5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG5" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1371,57 +1370,57 @@
       <c r="P6" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="Q6" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="R6" s="8" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="T6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="U6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="V6" s="8">
+        <v>81</v>
+      </c>
+      <c r="U6" s="8">
         <v>2013</v>
       </c>
+      <c r="V6" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="W6" s="8" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="X6" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z6" s="8">
+        <v>81</v>
+      </c>
+      <c r="Y6" s="8">
         <v>2013</v>
       </c>
+      <c r="Z6" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="AA6" s="8" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="AB6" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD6" s="8"/>
+        <v>81</v>
+      </c>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="AE6" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AF6" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG6" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH6" s="16" t="s">
+      <c r="AF6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG6" s="16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1470,57 +1469,57 @@
       <c r="P7" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="Q7" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="R7" s="7" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="T7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="U7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="V7" s="7">
+        <v>81</v>
+      </c>
+      <c r="U7" s="7">
         <v>2013</v>
       </c>
+      <c r="V7" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="W7" s="7" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z7" s="7">
+        <v>81</v>
+      </c>
+      <c r="Y7" s="7">
         <v>2013</v>
       </c>
+      <c r="Z7" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="AA7" s="7" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="AB7" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD7" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="AE7" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AF7" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG7" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH7" s="15" t="s">
+      <c r="AF7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG7" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1569,57 +1568,57 @@
       <c r="P8" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="Q8" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="R8" s="8" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="V8" s="8">
+        <v>81</v>
+      </c>
+      <c r="U8" s="8">
         <v>2013</v>
       </c>
+      <c r="V8" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="W8" s="8" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="X8" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y8" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z8" s="8">
+        <v>81</v>
+      </c>
+      <c r="Y8" s="8">
         <v>2013</v>
       </c>
+      <c r="Z8" s="8" t="s">
+        <v>81</v>
+      </c>
       <c r="AA8" s="8" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="AB8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="AC8" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD8" s="8"/>
+        <v>81</v>
+      </c>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="AE8" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AF8" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG8" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH8" s="16" t="s">
+      <c r="AF8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG8" s="16" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1668,57 +1667,57 @@
       <c r="P9" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="Q9" s="7" t="s">
+        <v>43</v>
+      </c>
       <c r="R9" s="7" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="T9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="U9" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="V9" s="7">
+        <v>81</v>
+      </c>
+      <c r="U9" s="7">
         <v>1979</v>
       </c>
+      <c r="V9" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="W9" s="7" t="s">
-        <v>81</v>
+        <v>49</v>
       </c>
       <c r="X9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y9" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z9" s="7">
+        <v>81</v>
+      </c>
+      <c r="Y9" s="7">
         <v>1979</v>
       </c>
+      <c r="Z9" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="AA9" s="7" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="AB9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC9" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD9" s="7"/>
+        <v>81</v>
+      </c>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="AE9" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AF9" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG9" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH9" s="15" t="s">
+      <c r="AF9" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG9" s="15" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1767,63 +1766,63 @@
       <c r="P10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="R10" s="9" t="s">
+      <c r="Q10" s="9" t="s">
         <v>43</v>
       </c>
+      <c r="R10" s="10" t="s">
+        <v>82</v>
+      </c>
       <c r="S10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="T10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="U10" s="9">
+        <v>1995</v>
+      </c>
+      <c r="V10" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="T10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="U10" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="V10" s="9">
+      <c r="W10" s="9">
         <v>1995</v>
       </c>
-      <c r="W10" s="10" t="s">
+      <c r="X10" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="X10" s="9">
+      <c r="Y10" s="10">
         <v>1995</v>
       </c>
-      <c r="Y10" s="10" t="s">
+      <c r="Z10" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA10" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB10" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="Z10" s="10">
-        <v>1995</v>
-      </c>
-      <c r="AA10" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB10" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AC10" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="11" t="s">
+        <v>85</v>
+      </c>
       <c r="AE10" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="AF10" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AG10" s="10" t="s">
+      <c r="AF10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="AH10" s="2" t="s">
+      <c r="AG10" s="2" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="S1:S1048576 U1:U1048576 W1:W1048576 AH1:AH1048576 Y1:Y1048576 AA1:AA1048576 AC1:AC1048576">
+  <conditionalFormatting sqref="R1:R1048576 T1:T1048576 V1:V1048576 AG1:AG1048576 X1:X1048576 Z1:Z1048576 AB1:AB1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="updated">
-      <formula>NOT(ISERROR(SEARCH("updated",S1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("updated",R1)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="filled in">
-      <formula>NOT(ISERROR(SEARCH("filled in",S1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("filled in",R1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>